<commit_message>
Schedule Changes & Updates
-Added Testcases to Phase IV of Development
-Fixed error in Gantt timeline with Phase III Usecases & Flowcharts. In
Illuminati_Dev_Timeline.pdf there is a one week deviation from the
expected due date in case of any issues regarding the usecase workload.
This has been updated in the Gantt Timeline.
-Expected completion of Usecase and flowcharts with deviation is the
week of April 3rd.
</commit_message>
<xml_diff>
--- a/Illuminati_Gantt_Timeline.xlsx
+++ b/Illuminati_Gantt_Timeline.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17830"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/57b83543f6faaf6c/Classes/2017 Spring CECS 343/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lilpe\OneDrive\Classes\2017 Spring CECS 343\Illuminati\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -86,9 +86,6 @@
     <t>Phase IV: Implementation &amp; Debugging</t>
   </si>
   <si>
-    <t>Gameplay Rules &amp; Functionality</t>
-  </si>
-  <si>
     <t>Art and Visual FX</t>
   </si>
   <si>
@@ -132,6 +129,9 @@
   </si>
   <si>
     <t>N, M</t>
+  </si>
+  <si>
+    <t>Gameplay Rules, Testcases, and Functionality</t>
   </si>
 </sst>
 </file>
@@ -451,7 +451,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -476,6 +476,36 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="12">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="4" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="15" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="14" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="8" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="8" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="9">
       <alignment vertical="center"/>
     </xf>
@@ -493,39 +523,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="4" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="15" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="14" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="8" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="8" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -1072,8 +1069,8 @@
   </sheetPr>
   <dimension ref="B1:O26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1095,77 +1092,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="15" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="2:15" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="16"/>
+        <v>24</v>
+      </c>
+      <c r="C2" s="9"/>
       <c r="E2" s="5"/>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="12"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="22"/>
       <c r="K2" s="6"/>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="12"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="22"/>
     </row>
     <row r="3" spans="2:15" s="4" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="23">
+      <c r="C3" s="16">
         <v>42779</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="16">
         <v>42786</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="17">
         <v>42793</v>
       </c>
-      <c r="F3" s="24">
+      <c r="F3" s="17">
         <v>42800</v>
       </c>
-      <c r="G3" s="24">
+      <c r="G3" s="17">
         <v>42807</v>
       </c>
-      <c r="H3" s="24">
+      <c r="H3" s="17">
         <v>42814</v>
       </c>
-      <c r="I3" s="24">
+      <c r="I3" s="17">
         <v>42821</v>
       </c>
-      <c r="J3" s="24">
+      <c r="J3" s="17">
         <v>42828</v>
       </c>
-      <c r="K3" s="24">
+      <c r="K3" s="17">
         <v>42835</v>
       </c>
-      <c r="L3" s="24">
+      <c r="L3" s="17">
         <v>42842</v>
       </c>
-      <c r="M3" s="24">
+      <c r="M3" s="17">
         <v>42849</v>
       </c>
-      <c r="N3" s="24">
+      <c r="N3" s="17">
         <v>42856</v>
       </c>
-      <c r="O3" s="24">
+      <c r="O3" s="17">
         <v>42863</v>
       </c>
     </row>
     <row r="4" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="9"/>
+      <c r="B4" s="19"/>
       <c r="C4" s="3">
         <v>1</v>
       </c>
@@ -1207,413 +1204,413 @@
       </c>
     </row>
     <row r="5" spans="2:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
     </row>
     <row r="6" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+    </row>
+    <row r="7" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+    </row>
+    <row r="8" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+    </row>
+    <row r="9" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+    </row>
+    <row r="10" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+    </row>
+    <row r="11" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="D11" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+    </row>
+    <row r="12" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+    </row>
+    <row r="13" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+    </row>
+    <row r="14" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+    </row>
+    <row r="15" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-      <c r="O6" s="19"/>
-    </row>
-    <row r="7" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="19"/>
-      <c r="O7" s="19"/>
-    </row>
-    <row r="8" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
-    </row>
-    <row r="9" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="17"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19"/>
-      <c r="O9" s="19"/>
-    </row>
-    <row r="10" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="19"/>
-    </row>
-    <row r="11" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-    </row>
-    <row r="12" spans="2:15" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="19"/>
-    </row>
-    <row r="13" spans="2:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
-      <c r="O13" s="19"/>
-    </row>
-    <row r="14" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19"/>
-      <c r="N14" s="19"/>
-      <c r="O14" s="19"/>
-    </row>
-    <row r="15" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="21" t="s">
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+    </row>
+    <row r="16" spans="2:15" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+    </row>
+    <row r="17" spans="2:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="12"/>
+    </row>
+    <row r="18" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="12"/>
+    </row>
+    <row r="19" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="12"/>
+    </row>
+    <row r="20" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="12"/>
+    </row>
+    <row r="21" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+    </row>
+    <row r="22" spans="2:15" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+    </row>
+    <row r="23" spans="2:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="O23" s="14"/>
+    </row>
+    <row r="24" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19"/>
-      <c r="N15" s="19"/>
-      <c r="O15" s="19"/>
-    </row>
-    <row r="16" spans="2:15" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
-      <c r="N16" s="19"/>
-      <c r="O16" s="19"/>
-    </row>
-    <row r="17" spans="2:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="21"/>
-      <c r="N17" s="21"/>
-      <c r="O17" s="19"/>
-    </row>
-    <row r="18" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="L18" s="21"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="21"/>
-      <c r="O18" s="19"/>
-    </row>
-    <row r="19" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="M19" s="21"/>
-      <c r="N19" s="21"/>
-      <c r="O19" s="19"/>
-    </row>
-    <row r="20" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="21"/>
-      <c r="O20" s="19"/>
-    </row>
-    <row r="21" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="21"/>
-      <c r="O21" s="21"/>
-    </row>
-    <row r="22" spans="2:15" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
-      <c r="N22" s="19"/>
-      <c r="O22" s="19"/>
-    </row>
-    <row r="23" spans="2:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="O23" s="21"/>
-    </row>
-    <row r="24" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="14" t="s">
+      <c r="O24" s="14"/>
+    </row>
+    <row r="25" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19"/>
-      <c r="M24" s="19"/>
-      <c r="N24" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="O24" s="21"/>
-    </row>
-    <row r="25" spans="2:15" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="19"/>
-      <c r="N25" s="19"/>
-      <c r="O25" s="21" t="s">
-        <v>26</v>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="14" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="2:15" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3"/>
@@ -1623,7 +1620,7 @@
     <mergeCell ref="F2:J2"/>
     <mergeCell ref="L2:O2"/>
   </mergeCells>
-  <conditionalFormatting sqref="D5:O25">
+  <conditionalFormatting sqref="D5:O12 D15:O25 D13:D14 F13:O14">
     <cfRule type="expression" dxfId="18" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -1690,13 +1687,13 @@
       <formula>C$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="7">
+  <dataValidations xWindow="497" yWindow="644" count="7">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A1"/>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="C2">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="E2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="K2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="K2 E13:E14"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter activity in column B, starting with cell B5_x000a_" sqref="B3:B4"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the project. Enter a new title in this cell. Highlight a period in H2. Chart legend is in J2 to AI2" sqref="B1"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select a period to highlight in H2. A Chart legend is in J2 to AI2" sqref="B2"/>

</xml_diff>